<commit_message>
crud citas terminado, filtros agregados
</commit_message>
<xml_diff>
--- a/results/excel/Usuarios.xlsx
+++ b/results/excel/Usuarios.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -110,82 +110,31 @@
     <t>TECNM</t>
   </si>
   <si>
-    <t>userPrueba2</t>
-  </si>
-  <si>
-    <t>usersillo2</t>
-  </si>
-  <si>
-    <t>apello1</t>
-  </si>
-  <si>
-    <t>apello2</t>
-  </si>
-  <si>
-    <t>user2P@gmail.com</t>
-  </si>
-  <si>
-    <t>124578</t>
-  </si>
-  <si>
-    <t>Guanajuato</t>
-  </si>
-  <si>
-    <t>flacow</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>jnn</t>
-  </si>
-  <si>
-    <t>kkk@gmail.com</t>
-  </si>
-  <si>
-    <t>156948</t>
-  </si>
-  <si>
-    <t>tecnm</t>
-  </si>
-  <si>
-    <t>buñuelos69</t>
-  </si>
-  <si>
-    <t>Omar Gadiel</t>
-  </si>
-  <si>
-    <t>Bolaños</t>
-  </si>
-  <si>
-    <t>García</t>
-  </si>
-  <si>
-    <t>omarbolanos198@gmail.com</t>
-  </si>
-  <si>
-    <t>4131060699</t>
-  </si>
-  <si>
-    <t>Beguña 107-B</t>
-  </si>
-  <si>
-    <t>wfef</t>
-  </si>
-  <si>
-    <t>ewfwe</t>
-  </si>
-  <si>
-    <t>frwefwef</t>
-  </si>
-  <si>
-    <t>wefwef</t>
-  </si>
-  <si>
-    <t>wefwefw</t>
+    <t>uker</t>
+  </si>
+  <si>
+    <t>miko</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>asdfghj</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -246,19 +195,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="3.94921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.00390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="10.1171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.9140625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="20.8828125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.29296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="24.5703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="10.9296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="21.1640625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="9.9296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -382,7 +331,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n" s="3">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="B5" t="s" s="3">
         <v>32</v>
@@ -400,10 +349,10 @@
         <v>36</v>
       </c>
       <c r="G5" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s" s="2">
         <v>37</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>38</v>
       </c>
       <c r="I5" t="s" s="2">
         <v>17</v>
@@ -411,88 +360,30 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="3">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="D6" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="H6" t="s" s="2">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="B7" t="s" s="3">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s" s="3">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s" s="3">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="I7" t="s" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="B8" t="s" s="3">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s" s="3">
-        <v>54</v>
-      </c>
-      <c r="D8" t="s" s="3">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s" s="3">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G8" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="I8" t="s" s="2">
         <v>17</v>
       </c>
     </row>

</xml_diff>